<commit_message>
More graphs wrt CN
</commit_message>
<xml_diff>
--- a/perftools/graphtools/kn-graphs-datamodel.xlsx
+++ b/perftools/graphtools/kn-graphs-datamodel.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="21900" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="21900" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="example table" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -493,6 +493,36 @@
   </si>
   <si>
     <t>npages (leeg op page-level, gevuld op run-level)</t>
+  </si>
+  <si>
+    <t>Voor 404's</t>
+  </si>
+  <si>
+    <t>topdomain</t>
+  </si>
+  <si>
+    <t>urlnoparams</t>
+  </si>
+  <si>
+    <t>status_code</t>
+  </si>
+  <si>
+    <t>error_code</t>
+  </si>
+  <si>
+    <t>task_succeed</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>sec_per_page</t>
+  </si>
+  <si>
+    <t>Influence on page loading time</t>
+  </si>
+  <si>
+    <t>only task_succeed = 1 has influence on reported page loading times.</t>
   </si>
 </sst>
 </file>
@@ -1384,17 +1414,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1404,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,12 +2123,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>